<commit_message>
Altura de peças padrão automaticamente
</commit_message>
<xml_diff>
--- a/output/pedidos.xlsx
+++ b/output/pedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,12 +518,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>250209_0001</t>
+          <t>250209_0003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>250209_0001_001</t>
+          <t>250209_0003_001</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -538,7 +538,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
         <v>1000</v>
@@ -561,27 +561,29 @@
         <v>500</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N2" t="n">
-        <v>341.82</v>
+        <v>205.75</v>
       </c>
       <c r="O2" t="n">
-        <v>341.82</v>
-      </c>
-      <c r="P2" t="n">
-        <v>655</v>
+        <v>102.88</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>kioj</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>250209_0001</t>
+          <t>250209_0003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>250209_0001_002</t>
+          <t>250209_0003_002</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -596,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -604,7 +606,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>1000</v>
@@ -619,27 +621,29 @@
         <v>550</v>
       </c>
       <c r="M3" t="n">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="N3" t="n">
-        <v>341.82</v>
+        <v>205.75</v>
       </c>
       <c r="O3" t="n">
-        <v>427.28</v>
-      </c>
-      <c r="P3" t="n">
-        <v>655</v>
+        <v>154.31</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>kioj</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>250209_0002</t>
+          <t>250209_0004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>250209_0002_001</t>
+          <t>250209_0004_001</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -662,19 +666,19 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="J4" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="K4" t="n">
-        <v>105</v>
+        <v>280</v>
       </c>
       <c r="L4" t="n">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="M4" t="n">
         <v>0.25</v>
@@ -685,19 +689,21 @@
       <c r="O4" t="n">
         <v>73.15000000000001</v>
       </c>
-      <c r="P4" t="n">
-        <v>655</v>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>kioj</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>250209_0003</t>
+          <t>250209_0005</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>250209_0003_001</t>
+          <t>250209_0005_001</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -712,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -720,7 +726,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
         <v>1000</v>
@@ -735,29 +741,29 @@
         <v>500</v>
       </c>
       <c r="M5" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>205.75</v>
+        <v>341.82</v>
       </c>
       <c r="O5" t="n">
-        <v>102.88</v>
+        <v>341.82</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>kioj</t>
+          <t>kjiko</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>250209_0003</t>
+          <t>250209_0005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>250209_0003_002</t>
+          <t>250209_0005_002</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -772,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -780,7 +786,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
         <v>1000</v>
@@ -795,29 +801,29 @@
         <v>550</v>
       </c>
       <c r="M6" t="n">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="N6" t="n">
-        <v>205.75</v>
+        <v>341.82</v>
       </c>
       <c r="O6" t="n">
-        <v>154.31</v>
+        <v>427.28</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>kioj</t>
+          <t>kjiko</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>250209_0004</t>
+          <t>250209_0006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>250209_0004_001</t>
+          <t>250209_0006_001</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -829,55 +835,55 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Peça Fixa - Vão</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="J7" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="K7" t="n">
-        <v>280</v>
+        <v>975</v>
       </c>
       <c r="L7" t="n">
-        <v>280</v>
+        <v>500</v>
       </c>
       <c r="M7" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N7" t="n">
-        <v>292.6</v>
+        <v>341.82</v>
       </c>
       <c r="O7" t="n">
-        <v>73.15000000000001</v>
+        <v>170.91</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>kioj</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>250209_0005</t>
+          <t>250209_0006</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>250209_0005_001</t>
+          <t>250209_0006_002</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -896,11 +902,11 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>1000</v>
@@ -909,35 +915,35 @@
         <v>1000</v>
       </c>
       <c r="K8" t="n">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="L8" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="N8" t="n">
         <v>341.82</v>
       </c>
       <c r="O8" t="n">
-        <v>341.82</v>
+        <v>256.36</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>kjiko</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>250209_0005</t>
+          <t>250209_0007</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>250209_0005_002</t>
+          <t>250209_0007_001</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -956,7 +962,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -969,35 +975,35 @@
         <v>1000</v>
       </c>
       <c r="K9" t="n">
-        <v>938</v>
+        <v>975</v>
       </c>
       <c r="L9" t="n">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="M9" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>341.82</v>
       </c>
       <c r="O9" t="n">
-        <v>427.28</v>
+        <v>341.82</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>kjiko</t>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>250209_0006</t>
+          <t>250209_0007</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>250209_0006_001</t>
+          <t>250209_0007_002</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1016,11 +1022,11 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
         <v>1000</v>
@@ -1029,35 +1035,35 @@
         <v>1000</v>
       </c>
       <c r="K10" t="n">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="L10" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="M10" t="n">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="N10" t="n">
         <v>341.82</v>
       </c>
       <c r="O10" t="n">
-        <v>170.91</v>
+        <v>427.28</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>250209_0006</t>
+          <t>250209_0008</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>250209_0006_002</t>
+          <t>250209_0008_001</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1069,55 +1075,55 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Principal</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="J11" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K11" t="n">
-        <v>938</v>
+        <v>100</v>
       </c>
       <c r="L11" t="n">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="M11" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="N11" t="n">
-        <v>341.82</v>
+        <v>436.14</v>
       </c>
       <c r="O11" t="n">
-        <v>256.36</v>
+        <v>109.04</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>250209_0007</t>
+          <t>250209_0009</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>250209_0007_001</t>
+          <t>250209_0009_001</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1140,7 +1146,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
         <v>1000</v>
@@ -1155,29 +1161,29 @@
         <v>500</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N12" t="n">
         <v>341.82</v>
       </c>
       <c r="O12" t="n">
-        <v>341.82</v>
+        <v>170.91</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>250209_0007</t>
+          <t>250209_0009</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>250209_0007_002</t>
+          <t>250209_0009_002</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1200,7 +1206,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
         <v>1000</v>
@@ -1215,29 +1221,29 @@
         <v>550</v>
       </c>
       <c r="M13" t="n">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="N13" t="n">
         <v>341.82</v>
       </c>
       <c r="O13" t="n">
-        <v>427.28</v>
+        <v>256.36</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>250209_0008</t>
+          <t>250210_0001</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>250209_0008_001</t>
+          <t>250210_0001_001</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1249,55 +1255,55 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Peça Principal</t>
+          <t>Peça Fixa - Vão</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="J14" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="K14" t="n">
-        <v>100</v>
+        <v>4980</v>
       </c>
       <c r="L14" t="n">
-        <v>500</v>
+        <v>680</v>
       </c>
       <c r="M14" t="n">
-        <v>0.25</v>
+        <v>3.5</v>
       </c>
       <c r="N14" t="n">
-        <v>436.14</v>
+        <v>348.29</v>
       </c>
       <c r="O14" t="n">
-        <v>109.04</v>
+        <v>1219.02</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>7845</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>250209_0009</t>
+          <t>250210_0002</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>250209_0009_001</t>
+          <t>250210_0002_001</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1312,7 +1318,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1323,41 +1329,41 @@
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="J15" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K15" t="n">
-        <v>975</v>
+        <v>1175</v>
       </c>
       <c r="L15" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M15" t="n">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="N15" t="n">
-        <v>341.82</v>
+        <v>483.79</v>
       </c>
       <c r="O15" t="n">
-        <v>170.91</v>
+        <v>604.74</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>7845</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>250209_0009</t>
+          <t>250210_0002</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>250209_0009_002</t>
+          <t>250210_0002_002</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1372,7 +1378,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1383,41 +1389,41 @@
         <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="J16" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K16" t="n">
-        <v>938</v>
+        <v>1138</v>
       </c>
       <c r="L16" t="n">
-        <v>550</v>
+        <v>1050</v>
       </c>
       <c r="M16" t="n">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="N16" t="n">
-        <v>341.82</v>
+        <v>483.79</v>
       </c>
       <c r="O16" t="n">
-        <v>256.36</v>
+        <v>604.74</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>7845</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>250210_0001</t>
+          <t>250210_0003</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>250210_0001_001</t>
+          <t>250210_0003_001</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1432,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1440,28 +1446,28 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
-        <v>5000</v>
+        <v>400</v>
       </c>
       <c r="J17" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="K17" t="n">
-        <v>4980</v>
+        <v>380</v>
       </c>
       <c r="L17" t="n">
-        <v>680</v>
+        <v>180</v>
       </c>
       <c r="M17" t="n">
-        <v>3.5</v>
+        <v>0.25</v>
       </c>
       <c r="N17" t="n">
-        <v>348.29</v>
+        <v>178.35</v>
       </c>
       <c r="O17" t="n">
-        <v>1219.02</v>
+        <v>44.59</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1472,12 +1478,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>250210_0002</t>
+          <t>250210_0004</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>250210_0002_001</t>
+          <t>250210_0004_001</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1489,55 +1495,55 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Fixa - Vão</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="J18" t="n">
-        <v>2000</v>
+        <v>750</v>
       </c>
       <c r="K18" t="n">
-        <v>1175</v>
+        <v>1380</v>
       </c>
       <c r="L18" t="n">
-        <v>1000</v>
+        <v>730</v>
       </c>
       <c r="M18" t="n">
         <v>1.25</v>
       </c>
       <c r="N18" t="n">
-        <v>483.79</v>
+        <v>264.63</v>
       </c>
       <c r="O18" t="n">
-        <v>604.74</v>
+        <v>330.79</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>7845</t>
+          <t>875</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>250210_0002</t>
+          <t>250210_0005</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>250210_0002_002</t>
+          <t>250210_0005_001</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1552,52 +1558,52 @@
         <v>7</v>
       </c>
       <c r="F19" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="J19" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="K19" t="n">
-        <v>1138</v>
+        <v>975</v>
       </c>
       <c r="L19" t="n">
-        <v>1050</v>
+        <v>500</v>
       </c>
       <c r="M19" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>483.79</v>
+        <v>332.75</v>
       </c>
       <c r="O19" t="n">
-        <v>604.74</v>
+        <v>332.75</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>7845</t>
+          <t>875</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>250210_0003</t>
+          <t>250210_0005</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>250210_0003_001</t>
+          <t>250210_0005_002</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1609,55 +1615,55 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Peça Fixa - Vão</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="J20" t="n">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="K20" t="n">
-        <v>380</v>
+        <v>938</v>
       </c>
       <c r="L20" t="n">
-        <v>180</v>
+        <v>550</v>
       </c>
       <c r="M20" t="n">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="N20" t="n">
-        <v>178.35</v>
+        <v>332.75</v>
       </c>
       <c r="O20" t="n">
-        <v>44.59</v>
+        <v>415.94</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>7845</t>
+          <t>875</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>250210_0004</t>
+          <t>250210_0006</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>250210_0004_001</t>
+          <t>250210_0006_001</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1672,7 +1678,7 @@
         <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1683,41 +1689,41 @@
         <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="J21" t="n">
-        <v>750</v>
+        <v>250</v>
       </c>
       <c r="K21" t="n">
-        <v>1380</v>
+        <v>480</v>
       </c>
       <c r="L21" t="n">
-        <v>730</v>
+        <v>230</v>
       </c>
       <c r="M21" t="n">
-        <v>1.25</v>
+        <v>0.25</v>
       </c>
       <c r="N21" t="n">
-        <v>264.63</v>
+        <v>297.78</v>
       </c>
       <c r="O21" t="n">
-        <v>330.79</v>
+        <v>74.44</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>875</t>
+          <t>4857896</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>250210_0005</t>
+          <t>250210_0007</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>250210_0005_001</t>
+          <t>250210_0007_001</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1732,7 +1738,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1758,26 +1764,26 @@
         <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>332.75</v>
+        <v>205.75</v>
       </c>
       <c r="O22" t="n">
-        <v>332.75</v>
+        <v>205.75</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>875</t>
+          <t>4857896</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>250210_0005</t>
+          <t>250210_0007</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>250210_0005_002</t>
+          <t>250210_0007_002</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1792,7 +1798,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1818,26 +1824,26 @@
         <v>1.25</v>
       </c>
       <c r="N23" t="n">
-        <v>332.75</v>
+        <v>205.75</v>
       </c>
       <c r="O23" t="n">
-        <v>415.94</v>
+        <v>257.19</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>875</t>
+          <t>4857896</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>250210_0006</t>
+          <t>250210_0008</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>250210_0006_001</t>
+          <t>250210_0008_001</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1849,55 +1855,55 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Peça Fixa - Vão</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K24" t="n">
+        <v>975</v>
+      </c>
+      <c r="L24" t="n">
         <v>500</v>
       </c>
-      <c r="J24" t="n">
-        <v>250</v>
-      </c>
-      <c r="K24" t="n">
-        <v>480</v>
-      </c>
-      <c r="L24" t="n">
-        <v>230</v>
-      </c>
       <c r="M24" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>297.78</v>
+        <v>205.75</v>
       </c>
       <c r="O24" t="n">
-        <v>74.44</v>
+        <v>205.75</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>4857896</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>250210_0007</t>
+          <t>250210_0008</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>250210_0007_001</t>
+          <t>250210_0008_002</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1916,7 +1922,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1929,35 +1935,35 @@
         <v>1000</v>
       </c>
       <c r="K25" t="n">
-        <v>975</v>
+        <v>938</v>
       </c>
       <c r="L25" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="M25" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="N25" t="n">
         <v>205.75</v>
       </c>
       <c r="O25" t="n">
-        <v>205.75</v>
+        <v>257.19</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>4857896</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>250210_0007</t>
+          <t>250210_0009</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>250210_0007_002</t>
+          <t>250210_0009_001</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1969,55 +1975,55 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Fixa - Vão</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J26" t="n">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="K26" t="n">
-        <v>938</v>
+        <v>1480</v>
       </c>
       <c r="L26" t="n">
-        <v>550</v>
+        <v>380</v>
       </c>
       <c r="M26" t="n">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="N26" t="n">
-        <v>205.75</v>
+        <v>264.63</v>
       </c>
       <c r="O26" t="n">
-        <v>257.19</v>
+        <v>198.47</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>4857896</t>
+          <t>456</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>250210_0008</t>
+          <t>250211_0001</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>250210_0008_001</t>
+          <t>250211_0001_001</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -2029,55 +2035,55 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F27" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Principal</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="J27" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="K27" t="n">
-        <v>975</v>
+        <v>100</v>
       </c>
       <c r="L27" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="M27" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="N27" t="n">
-        <v>205.75</v>
+        <v>341.82</v>
       </c>
       <c r="O27" t="n">
-        <v>205.75</v>
+        <v>85.45999999999999</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>45</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>250210_0008</t>
+          <t>250211_0002</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>250210_0008_002</t>
+          <t>250211_0002_001</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -2089,14 +2095,14 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Fixa - Vão</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -2109,19 +2115,19 @@
         <v>1000</v>
       </c>
       <c r="K28" t="n">
-        <v>938</v>
+        <v>980</v>
       </c>
       <c r="L28" t="n">
-        <v>550</v>
+        <v>980</v>
       </c>
       <c r="M28" t="n">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="N28" t="n">
-        <v>205.75</v>
+        <v>292.6</v>
       </c>
       <c r="O28" t="n">
-        <v>257.19</v>
+        <v>585.2</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -2132,12 +2138,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>250210_0009</t>
+          <t>250211_0003</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>250210_0009_001</t>
+          <t>250211_0003_001</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -2149,55 +2155,55 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Peça Fixa - Vão</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="J29" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="K29" t="n">
-        <v>1480</v>
+        <v>975</v>
       </c>
       <c r="L29" t="n">
-        <v>380</v>
+        <v>500</v>
       </c>
       <c r="M29" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="N29" t="n">
-        <v>264.63</v>
+        <v>341.82</v>
       </c>
       <c r="O29" t="n">
-        <v>198.47</v>
+        <v>170.91</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>hujilo</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>250211_0001</t>
+          <t>250211_0003</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>250211_0001_001</t>
+          <t>250211_0003_002</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -2209,55 +2215,55 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>11</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Peça Principal</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>1</v>
       </c>
       <c r="I30" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="J30" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="K30" t="n">
-        <v>100</v>
+        <v>938</v>
       </c>
       <c r="L30" t="n">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="M30" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="N30" t="n">
         <v>341.82</v>
       </c>
       <c r="O30" t="n">
-        <v>85.45999999999999</v>
+        <v>256.36</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>hujilo</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>250211_0002</t>
+          <t>250211_0004</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>250211_0002_001</t>
+          <t>250211_0004_001</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -2269,55 +2275,55 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Peça Fixa - Vão</t>
+          <t>Peça Principal</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="J31" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="K31" t="n">
-        <v>980</v>
+        <v>100</v>
       </c>
       <c r="L31" t="n">
-        <v>980</v>
+        <v>100</v>
       </c>
       <c r="M31" t="n">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="N31" t="n">
-        <v>292.6</v>
+        <v>312</v>
       </c>
       <c r="O31" t="n">
-        <v>585.2</v>
+        <v>78</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>hujilo</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>250211_0003</t>
+          <t>250211_0005</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>250211_0003_001</t>
+          <t>250211_0005_001</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -2329,39 +2335,39 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F32" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Peça Fixa</t>
+          <t>Peça Principal</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" t="n">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="J32" t="n">
-        <v>1000</v>
+        <v>45</v>
       </c>
       <c r="K32" t="n">
-        <v>975</v>
+        <v>50</v>
       </c>
       <c r="L32" t="n">
-        <v>500</v>
+        <v>45</v>
       </c>
       <c r="M32" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N32" t="n">
-        <v>341.82</v>
+        <v>332.75</v>
       </c>
       <c r="O32" t="n">
-        <v>170.91</v>
+        <v>83.19</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -2372,12 +2378,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>250211_0003</t>
+          <t>250211_0006</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>250211_0003_002</t>
+          <t>250211_0006_001</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -2396,7 +2402,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Peça Móvel</t>
+          <t>Peça Fixa</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -2409,35 +2415,35 @@
         <v>1000</v>
       </c>
       <c r="K33" t="n">
-        <v>938</v>
+        <v>975</v>
       </c>
       <c r="L33" t="n">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="M33" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="N33" t="n">
         <v>341.82</v>
       </c>
       <c r="O33" t="n">
-        <v>256.36</v>
+        <v>170.91</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>hujilo</t>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>250211_0004</t>
+          <t>250211_0006</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>250211_0004_001</t>
+          <t>250211_0006_002</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -2449,55 +2455,55 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Peça Principal</t>
+          <t>Peça Móvel</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="J34" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="K34" t="n">
-        <v>100</v>
+        <v>938</v>
       </c>
       <c r="L34" t="n">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="M34" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="N34" t="n">
-        <v>312</v>
+        <v>341.82</v>
       </c>
       <c r="O34" t="n">
-        <v>78</v>
+        <v>256.36</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>hujilo</t>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>250211_0005</t>
+          <t>250212_0001</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>250211_0005_001</t>
+          <t>250212_0001_001</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -2509,43 +2515,343 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
+        <v>11</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Peça Fixa</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K35" t="n">
+        <v>975</v>
+      </c>
+      <c r="L35" t="n">
+        <v>500</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N35" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O35" t="n">
+        <v>170.91</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>47845</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>250212_0001</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>250212_0001_002</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>7</v>
+      </c>
+      <c r="F36" t="n">
+        <v>11</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Peça Móvel</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K36" t="n">
+        <v>938</v>
+      </c>
+      <c r="L36" t="n">
+        <v>550</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="N36" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O36" t="n">
+        <v>256.36</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>47845</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>250212_0002</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>250212_0002_001</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>28</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1845</v>
+      </c>
+      <c r="J37" t="n">
+        <v>700</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1845</v>
+      </c>
+      <c r="L37" t="n">
+        <v>700</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N37" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O37" t="n">
+        <v>308.62</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>47845</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>250212_0003</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>250212_0003_001</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>68</v>
+      </c>
+      <c r="F38" t="n">
         <v>20</v>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>Peça Principal</t>
         </is>
       </c>
-      <c r="H35" t="n">
-        <v>2</v>
-      </c>
-      <c r="I35" t="n">
-        <v>50</v>
-      </c>
-      <c r="J35" t="n">
-        <v>45</v>
-      </c>
-      <c r="K35" t="n">
-        <v>50</v>
-      </c>
-      <c r="L35" t="n">
-        <v>45</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="N35" t="n">
+      <c r="H38" t="n">
+        <v>3</v>
+      </c>
+      <c r="I38" t="n">
+        <v>975</v>
+      </c>
+      <c r="J38" t="n">
+        <v>600</v>
+      </c>
+      <c r="K38" t="n">
+        <v>975</v>
+      </c>
+      <c r="L38" t="n">
+        <v>600</v>
+      </c>
+      <c r="M38" t="n">
+        <v>2</v>
+      </c>
+      <c r="N38" t="n">
         <v>332.75</v>
       </c>
-      <c r="O35" t="n">
-        <v>83.19</v>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>hujilo</t>
+      <c r="O38" t="n">
+        <v>665.5</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>47845</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>250212_0004</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>250212_0004_001</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" t="n">
+        <v>980</v>
+      </c>
+      <c r="J39" t="n">
+        <v>475</v>
+      </c>
+      <c r="K39" t="n">
+        <v>980</v>
+      </c>
+      <c r="L39" t="n">
+        <v>475</v>
+      </c>
+      <c r="M39" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N39" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O39" t="n">
+        <v>514.38</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>47845</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>250212_0005</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>250212_0005_001</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>12</v>
+      </c>
+      <c r="F40" t="n">
+        <v>12</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>3</v>
+      </c>
+      <c r="I40" t="n">
+        <v>500</v>
+      </c>
+      <c r="J40" t="n">
+        <v>300</v>
+      </c>
+      <c r="K40" t="n">
+        <v>500</v>
+      </c>
+      <c r="L40" t="n">
+        <v>300</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N40" t="n">
+        <v>483.79</v>
+      </c>
+      <c r="O40" t="n">
+        <v>241.9</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Faue</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionando valores nos pedidos
</commit_message>
<xml_diff>
--- a/output/pedidos.xlsx
+++ b/output/pedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2855,6 +2855,546 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>250213_0001</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>250213_0001_001</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>8</v>
+      </c>
+      <c r="F41" t="n">
+        <v>11</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Peça Fixa</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K41" t="n">
+        <v>975</v>
+      </c>
+      <c r="L41" t="n">
+        <v>500</v>
+      </c>
+      <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O41" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>250213_0001</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>250213_0001_002</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>8</v>
+      </c>
+      <c r="F42" t="n">
+        <v>11</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Peça Móvel</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>2</v>
+      </c>
+      <c r="I42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K42" t="n">
+        <v>938</v>
+      </c>
+      <c r="L42" t="n">
+        <v>550</v>
+      </c>
+      <c r="M42" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="N42" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O42" t="n">
+        <v>427.28</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>250213_0002</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>250213_0002_001</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>39</v>
+      </c>
+      <c r="F43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1880</v>
+      </c>
+      <c r="J43" t="n">
+        <v>550</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1880</v>
+      </c>
+      <c r="L43" t="n">
+        <v>550</v>
+      </c>
+      <c r="M43" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="N43" t="n">
+        <v>332.75</v>
+      </c>
+      <c r="O43" t="n">
+        <v>748.6900000000001</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>250213_0003</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>250213_0003_001</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>26</v>
+      </c>
+      <c r="F44" t="n">
+        <v>11</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1845</v>
+      </c>
+      <c r="J44" t="n">
+        <v>600</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1845</v>
+      </c>
+      <c r="L44" t="n">
+        <v>600</v>
+      </c>
+      <c r="M44" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="N44" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O44" t="n">
+        <v>427.28</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>78945</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>250213_0004</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>250213_0004_001</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>29</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1845</v>
+      </c>
+      <c r="J45" t="n">
+        <v>750</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1845</v>
+      </c>
+      <c r="L45" t="n">
+        <v>750</v>
+      </c>
+      <c r="M45" t="n">
+        <v>7</v>
+      </c>
+      <c r="N45" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1440.25</v>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>78945</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>250213_0005</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>250213_0005_001</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>42</v>
+      </c>
+      <c r="F46" t="n">
+        <v>11</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>3</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1880</v>
+      </c>
+      <c r="J46" t="n">
+        <v>700</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1880</v>
+      </c>
+      <c r="L46" t="n">
+        <v>700</v>
+      </c>
+      <c r="M46" t="n">
+        <v>4</v>
+      </c>
+      <c r="N46" t="n">
+        <v>341.82</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1367.28</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>kijk</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>250213_0006</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>250213_0006_001</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>51</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>938</v>
+      </c>
+      <c r="J47" t="n">
+        <v>450</v>
+      </c>
+      <c r="K47" t="n">
+        <v>938</v>
+      </c>
+      <c r="L47" t="n">
+        <v>450</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N47" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O47" t="n">
+        <v>102.88</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>kijk</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>250213_0007</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>250213_0007_001</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>41</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1880</v>
+      </c>
+      <c r="J48" t="n">
+        <v>650</v>
+      </c>
+      <c r="K48" t="n">
+        <v>1880</v>
+      </c>
+      <c r="L48" t="n">
+        <v>650</v>
+      </c>
+      <c r="M48" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="N48" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O48" t="n">
+        <v>257.19</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Boxes casa</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>250213_0008</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>250213_0008_001</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>DOUGLAS</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>42</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Peça Principal</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1880</v>
+      </c>
+      <c r="J49" t="n">
+        <v>700</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1880</v>
+      </c>
+      <c r="L49" t="n">
+        <v>700</v>
+      </c>
+      <c r="M49" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N49" t="n">
+        <v>205.75</v>
+      </c>
+      <c r="O49" t="n">
+        <v>308.62</v>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Boxes casa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando regiao no pedido
</commit_message>
<xml_diff>
--- a/output/pedidos.xlsx
+++ b/output/pedidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\OneDrive\Área de Trabalho\python-whatsapp\chatbot\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8F719D-05FD-4019-BB2D-0EBB439F0786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8C21ED-0612-48A1-8A97-CDD8C7E37189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>id_pedido</t>
   </si>
@@ -79,6 +79,9 @@
     <t>status_pedido</t>
   </si>
   <si>
+    <t>regiao</t>
+  </si>
+  <si>
     <t>250219_0001</t>
   </si>
   <si>
@@ -194,6 +197,30 @@
   </si>
   <si>
     <t>FIXO [FINAL]</t>
+  </si>
+  <si>
+    <t>250219_0009</t>
+  </si>
+  <si>
+    <t>250219_0009_001</t>
+  </si>
+  <si>
+    <t>CLIENTE 6</t>
+  </si>
+  <si>
+    <t>box fume</t>
+  </si>
+  <si>
+    <t>250219_0010</t>
+  </si>
+  <si>
+    <t>250219_0010_001</t>
+  </si>
+  <si>
+    <t>ghj</t>
+  </si>
+  <si>
+    <t>VERDE</t>
   </si>
 </sst>
 </file>
@@ -556,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,23 +595,24 @@
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,580 +626,704 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
         <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="J2" t="s">
+        <v>25</v>
       </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>1845</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>450</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1845</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>450</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
       <c r="P2">
-        <v>341.82</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>341.82</v>
       </c>
-      <c r="R2" t="s">
-        <v>25</v>
+      <c r="R2">
+        <v>341.82</v>
       </c>
       <c r="S2" t="s">
         <v>26</v>
       </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3">
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3">
         <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1845</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>400</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1845</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>400</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>6</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>341.82</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2050.92</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
       </c>
       <c r="S3" t="s">
         <v>31</v>
       </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
       <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
         <v>8</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1880</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>600</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1880</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>600</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>9.25</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>332.75</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>3077.94</v>
-      </c>
-      <c r="R4" t="s">
-        <v>30</v>
       </c>
       <c r="S4" t="s">
         <v>31</v>
       </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
       <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
       </c>
       <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>1845</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>600</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1845</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>600</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>1.25</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>205.75</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>257.19</v>
       </c>
-      <c r="R5" t="s">
-        <v>40</v>
-      </c>
       <c r="S5" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="T5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
         <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6">
-        <v>1</v>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
       <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>1845</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>550</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1845</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>550</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1.25</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>341.82</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>427.28</v>
       </c>
-      <c r="R6" t="s">
-        <v>44</v>
-      </c>
       <c r="S6" t="s">
-        <v>31</v>
+        <v>45</v>
+      </c>
+      <c r="T6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7">
+      <c r="F7">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
       <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1845</v>
+      </c>
+      <c r="M7">
+        <v>400</v>
+      </c>
+      <c r="N7">
+        <v>1845</v>
+      </c>
+      <c r="O7">
+        <v>400</v>
+      </c>
+      <c r="P7">
+        <v>0.75</v>
+      </c>
+      <c r="Q7">
+        <v>332.75</v>
+      </c>
+      <c r="R7">
+        <v>249.56</v>
+      </c>
+      <c r="S7" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1845</v>
-      </c>
-      <c r="L7">
-        <v>400</v>
-      </c>
-      <c r="M7">
-        <v>1845</v>
-      </c>
-      <c r="N7">
-        <v>400</v>
-      </c>
-      <c r="O7">
-        <v>0.75</v>
-      </c>
-      <c r="P7">
-        <v>332.75</v>
-      </c>
-      <c r="Q7">
-        <v>249.56</v>
-      </c>
-      <c r="R7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1000</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1700</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>975</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>425</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
       <c r="P8">
-        <v>341.82</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>341.82</v>
       </c>
-      <c r="R8" t="s">
-        <v>52</v>
+      <c r="R8">
+        <v>341.82</v>
       </c>
       <c r="S8" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="T8" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9">
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
       <c r="I9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1000</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1700</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>938</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>475</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
       <c r="P9">
-        <v>341.82</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <v>341.82</v>
       </c>
-      <c r="R9" t="s">
-        <v>52</v>
+      <c r="R9">
+        <v>341.82</v>
       </c>
       <c r="S9" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="T9" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10">
         <v>20</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>500</v>
+      </c>
+      <c r="M10">
+        <v>800</v>
+      </c>
+      <c r="N10">
+        <v>500</v>
+      </c>
+      <c r="O10">
+        <v>800</v>
+      </c>
+      <c r="P10">
+        <v>0.5</v>
+      </c>
+      <c r="Q10">
+        <v>332.75</v>
+      </c>
+      <c r="R10">
+        <v>166.38</v>
+      </c>
+      <c r="S10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1845</v>
+      </c>
+      <c r="M11">
+        <v>450</v>
+      </c>
+      <c r="N11">
+        <v>1845</v>
+      </c>
+      <c r="O11">
+        <v>450</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>341.82</v>
+      </c>
+      <c r="R11">
+        <v>341.82</v>
+      </c>
+      <c r="S11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
         <v>35</v>
       </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>500</v>
-      </c>
-      <c r="L10">
-        <v>800</v>
-      </c>
-      <c r="M10">
-        <v>500</v>
-      </c>
-      <c r="N10">
-        <v>800</v>
-      </c>
-      <c r="O10">
-        <v>0.5</v>
-      </c>
-      <c r="P10">
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1880</v>
+      </c>
+      <c r="M12">
+        <v>600</v>
+      </c>
+      <c r="N12">
+        <v>1880</v>
+      </c>
+      <c r="O12">
+        <v>600</v>
+      </c>
+      <c r="P12">
+        <v>1.25</v>
+      </c>
+      <c r="Q12">
         <v>332.75</v>
       </c>
-      <c r="Q10">
-        <v>166.38</v>
-      </c>
-      <c r="R10" t="s">
-        <v>52</v>
-      </c>
-      <c r="S10" t="s">
-        <v>26</v>
+      <c r="R12">
+        <v>415.94</v>
+      </c>
+      <c r="S12" t="s">
+        <v>65</v>
+      </c>
+      <c r="T12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arrumando bug quando cliente não tem orçamento
</commit_message>
<xml_diff>
--- a/output/pedidos.xlsx
+++ b/output/pedidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\OneDrive\Área de Trabalho\python-whatsapp\chatbot\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8C21ED-0612-48A1-8A97-CDD8C7E37189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47071597-71A3-4B7C-9AC2-87C84E79C89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
   <si>
     <t>id_pedido</t>
   </si>
@@ -34,6 +34,9 @@
     <t>nome_cliente</t>
   </si>
   <si>
+    <t>regiao</t>
+  </si>
+  <si>
     <t>id_projeto</t>
   </si>
   <si>
@@ -79,7 +82,10 @@
     <t>status_pedido</t>
   </si>
   <si>
-    <t>regiao</t>
+    <t>data_orcamento</t>
+  </si>
+  <si>
+    <t>data_pedido</t>
   </si>
   <si>
     <t>250219_0001</t>
@@ -217,10 +223,43 @@
     <t>250219_0010_001</t>
   </si>
   <si>
+    <t>VERDE</t>
+  </si>
+  <si>
     <t>ghj</t>
   </si>
   <si>
-    <t>VERDE</t>
+    <t>250219_0011</t>
+  </si>
+  <si>
+    <t>250219_0011_001</t>
+  </si>
+  <si>
+    <t>BOX PADRÃO - MÓVEL - 750MM</t>
+  </si>
+  <si>
+    <t>huejia</t>
+  </si>
+  <si>
+    <t>2025-02-19 22:24:48</t>
+  </si>
+  <si>
+    <t>2025-02-19 22:25:26</t>
+  </si>
+  <si>
+    <t>250219_0012</t>
+  </si>
+  <si>
+    <t>250219_0012_001</t>
+  </si>
+  <si>
+    <t>JANELA PADRÃO - MÓVEL - 800MM</t>
+  </si>
+  <si>
+    <t>vvaiau</t>
+  </si>
+  <si>
+    <t>2025-02-19 22:26:19</t>
   </si>
 </sst>
 </file>
@@ -583,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,9 +649,10 @@
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,81 +666,87 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -727,39 +773,39 @@
         <v>341.82</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>8</v>
@@ -786,39 +832,39 @@
         <v>2050.92</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K4">
         <v>8</v>
@@ -845,39 +891,39 @@
         <v>3077.94</v>
       </c>
       <c r="S4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -904,39 +950,39 @@
         <v>257.19</v>
       </c>
       <c r="S5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H6">
         <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -963,39 +1009,39 @@
         <v>427.28</v>
       </c>
       <c r="S6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1022,39 +1068,39 @@
         <v>249.56</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="T7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1081,39 +1127,39 @@
         <v>341.82</v>
       </c>
       <c r="S8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1140,39 +1186,39 @@
         <v>341.82</v>
       </c>
       <c r="S9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H10">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1199,39 +1245,39 @@
         <v>166.38</v>
       </c>
       <c r="S10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H11">
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1258,42 +1304,42 @@
         <v>341.82</v>
       </c>
       <c r="S11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H12">
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1320,10 +1366,146 @@
         <v>415.94</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="T12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
         <v>27</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>1880</v>
+      </c>
+      <c r="M13">
+        <v>750</v>
+      </c>
+      <c r="N13">
+        <v>1880</v>
+      </c>
+      <c r="O13">
+        <v>750</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>341.82</v>
+      </c>
+      <c r="R13">
+        <v>1025.46</v>
+      </c>
+      <c r="S13" t="s">
+        <v>72</v>
+      </c>
+      <c r="T13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>975</v>
+      </c>
+      <c r="M14">
+        <v>800</v>
+      </c>
+      <c r="N14">
+        <v>975</v>
+      </c>
+      <c r="O14">
+        <v>800</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>205.75</v>
+      </c>
+      <c r="R14">
+        <v>205.75</v>
+      </c>
+      <c r="S14" t="s">
+        <v>78</v>
+      </c>
+      <c r="T14" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" t="s">
+        <v>79</v>
+      </c>
+      <c r="V14" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tempo de resposta do bot aumentado
</commit_message>
<xml_diff>
--- a/output/pedidos.xlsx
+++ b/output/pedidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\OneDrive\Área de Trabalho\python-whatsapp\chatbot\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47071597-71A3-4B7C-9AC2-87C84E79C89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A9E8B9-60D8-4C82-A0F6-C06E48133469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>id_pedido</t>
   </si>
@@ -229,6 +229,9 @@
     <t>ghj</t>
   </si>
   <si>
+    <t>2025-02-19 22:34:44</t>
+  </si>
+  <si>
     <t>250219_0011</t>
   </si>
   <si>
@@ -260,6 +263,24 @@
   </si>
   <si>
     <t>2025-02-19 22:26:19</t>
+  </si>
+  <si>
+    <t>250220_0001</t>
+  </si>
+  <si>
+    <t>250220_0001_001</t>
+  </si>
+  <si>
+    <t>BOX PADRÃO - FIXO - 750MM</t>
+  </si>
+  <si>
+    <t>465</t>
+  </si>
+  <si>
+    <t>CANCELADO</t>
+  </si>
+  <si>
+    <t>2025-02-20 00:21:19</t>
   </si>
 </sst>
 </file>
@@ -622,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,15 +1390,18 @@
         <v>68</v>
       </c>
       <c r="T12" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="V12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -1392,7 +1416,7 @@
         <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H13">
         <v>11</v>
@@ -1428,24 +1452,24 @@
         <v>1025.46</v>
       </c>
       <c r="S13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T13" t="s">
         <v>34</v>
       </c>
       <c r="U13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="V13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -1460,7 +1484,7 @@
         <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1496,16 +1520,81 @@
         <v>205.75</v>
       </c>
       <c r="S14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T14" t="s">
         <v>34</v>
       </c>
       <c r="U14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V14" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1845</v>
+      </c>
+      <c r="M15">
+        <v>750</v>
+      </c>
+      <c r="N15">
+        <v>1845</v>
+      </c>
+      <c r="O15">
+        <v>750</v>
+      </c>
+      <c r="P15">
+        <v>1.5</v>
+      </c>
+      <c r="Q15">
+        <v>332.75</v>
+      </c>
+      <c r="R15">
+        <v>499.12</v>
+      </c>
+      <c r="S15" t="s">
+        <v>84</v>
+      </c>
+      <c r="T15" t="s">
+        <v>85</v>
+      </c>
+      <c r="U15" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>